<commit_message>
updating ToDolist & planning CanvasAd flow
</commit_message>
<xml_diff>
--- a/작업 필요 리스트업.xlsx
+++ b/작업 필요 리스트업.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>현상 (as-is)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +60,47 @@
   </si>
   <si>
     <t>dialog.csv 에서 level2 level3 을 로드하고 싶음 (그래서 쥬김 루트에서는 level2 를 계속 부르려고요)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스와 충돌 체크 해서 대미지 입히도록 수정한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스 처치 즉시 스토리가 나오는데 스토리가 나오면 이동 입력이 먹지 않아서 
+보스의 잔여 공격을 맞고 죽을 수 밖에 없는 현상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스가 처치되는 즉시 보스의 프로젝타일들을 객체 파괴 리스트에 넣어서 삭제한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광고 페이지가 띄워지는 경우, 스토리 창은 hide 시킨다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스 객체와 충돌 시 대미지를 입지 않음 &lt;그림1 참조)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토리가 나오고 나서 죽게 되는 경우, 스토리 창 위에 광고 페이지가 걸리는 현상 &lt;그림2&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안드로이드 빌드 변경 후 StartMenu 가 까맣게 나오는 현상</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -93,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +144,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,7 +183,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -146,14 +193,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -170,6 +223,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2409531</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152017</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="4676775"/>
+          <a:ext cx="2352381" cy="3066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2190476</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>75745</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="7800975"/>
+          <a:ext cx="2190476" cy="3638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,15 +593,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="74.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="101.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
   </cols>
@@ -486,86 +620,110 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
@@ -601,7 +759,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -641,7 +799,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -656,11 +814,22 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>